<commit_message>
day_4 has been started
</commit_message>
<xml_diff>
--- a/European_Coaching/day_3/excel/task-2.xlsx
+++ b/European_Coaching/day_3/excel/task-2.xlsx
@@ -105,18 +105,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,80 +455,103 @@
   </cols>
   <sheetData>
     <row r="4" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="5:13" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="F5" s="5" t="s">
+    <row r="5" spans="5:13" ht="36" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="11">
         <v>37426</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="10">
         <f ca="1">DATEDIF(G8,TODAY(),"Y")</f>
         <v>23</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="10">
         <f ca="1">DATEDIF(G8,TODAY(),"M")</f>
         <v>277</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="10">
         <f ca="1">DATEDIF(G8,TODAY(),"D")</f>
         <v>8435</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K8" s="10" t="str">
         <f ca="1">IF(H8&gt;17,"YOU ARE VOTER",IF(H8&lt;18,"YOU ARE NON VOTER"))</f>
         <v>YOU ARE VOTER</v>
       </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="H9">
+      <c r="E9" s="1"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
         <f ca="1">DATEDIF(G8,TODAY(),"Y")</f>
         <v>23</v>
       </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>